<commit_message>
Documentation mise à jour
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -350,6 +350,40 @@
     <t>Pour le 14 Mars proposer un projet TPI
 Partir sur un RTS
 avoir un solution Tower Defense au cas ou</t>
+  </si>
+  <si>
+    <t>Mail Chef de Projet</t>
+  </si>
+  <si>
+    <t>mal entendu de ma part concernant la partie adaptative du pathfinding
+prévu initialement : un labyrinth: cela ne casse rien au niveau de ce qui a été mis en place, sa mise en place va impacter des modules qui sont encore à implémenter</t>
+  </si>
+  <si>
+    <t>Analyse et Conception
+Pathfinding Labyrinth</t>
+  </si>
+  <si>
+    <t>Problématique et intégration aux grid générics déjà en place</t>
+  </si>
+  <si>
+    <t>Redirection des objectifs</t>
+  </si>
+  <si>
+    <t>La réponse au mail concernant la demande pour éviter la détection d'obstacle a été reçu.
+Cependant ne restant que 3 semaines il est urgent de définir les objectifs afin d'avoir un projet qui remplisse un maximum le cahier des charges</t>
+  </si>
+  <si>
+    <t>Mettre la documentation technique à jour</t>
+  </si>
+  <si>
+    <t>Analyse et conception
+Pathfinding Detection chemin bloqué</t>
+  </si>
+  <si>
+    <t>https://www.redblobgames.com/pathfinding/a-star/introduction.html</t>
+  </si>
+  <si>
+    <t>Recherche via RedBlobGame contenant enormement d'article et lien d'articles sur le pathfinding</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1376,7 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,65 +2268,113 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+    <row r="40" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>44621</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.49583333333333335</v>
+      </c>
       <c r="D40" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="21"/>
+        <v>9.7222222222222432E-3</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="G40" s="6"/>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
+      <c r="A41" s="31">
+        <v>44621</v>
+      </c>
+      <c r="B41" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="C41" s="18">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D41" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="23"/>
+        <v>1.4583333333333282E-2</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="G41" s="19"/>
       <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="3">
+        <v>44621</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.57847222222222217</v>
+      </c>
       <c r="D42" s="4">
         <f t="shared" ref="D42:D81" si="7">C42-B42</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="6"/>
+        <v>1.5972222222222165E-2</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="31">
+        <v>44621</v>
+      </c>
+      <c r="B43" s="18">
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="C43" s="18">
+        <v>0.62916666666666665</v>
+      </c>
       <c r="D43" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="30"/>
+        <v>5.0694444444444486E-2</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>87</v>
+      </c>
       <c r="F43" s="23"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="20"/>
+      <c r="G43" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
+      <c r="A44" s="3">
+        <v>44621</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.64236111111111105</v>
+      </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-0.64236111111111105</v>
       </c>
       <c r="E44" s="30"/>
       <c r="F44" s="21"/>

</xml_diff>

<commit_message>
Mise à jour documentation
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="133">
   <si>
     <t>Date</t>
   </si>
@@ -504,6 +504,27 @@
   </si>
   <si>
     <t>On arrive enfin au bout de l'implémentation! Le code peut être mise dans le projet principal, cependant il faut encore un système de A* pour detecter si un chemin est possible</t>
+  </si>
+  <si>
+    <t>Refactor</t>
+  </si>
+  <si>
+    <t>refactor Astar pathfinding</t>
+  </si>
+  <si>
+    <t>implémentation de Astar
+Pathfinding</t>
+  </si>
+  <si>
+    <t>PROBLEME : la grille doit s'adapter a une grille plus grande..</t>
+  </si>
+  <si>
+    <t>Analyse du problème d'adaptation de grille</t>
+  </si>
+  <si>
+    <t>Problematique : 
+Soit on calcule dynamiquement a chaque besoin les cellule concernée
+on crée une grille temporaire adapté qui calculera une fois lors du callback tout les cas</t>
   </si>
 </sst>
 </file>
@@ -1495,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,52 +2966,84 @@
       <c r="B64" s="4">
         <v>0.65902777777777777</v>
       </c>
-      <c r="C64" s="4"/>
+      <c r="C64" s="4">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D64" s="4">
         <f t="shared" si="7"/>
-        <v>-0.65902777777777777</v>
-      </c>
-      <c r="E64" s="30"/>
+        <v>4.5833333333333393E-2</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>127</v>
+      </c>
       <c r="F64" s="21"/>
       <c r="G64" s="6"/>
       <c r="H64" s="9"/>
     </row>
     <row r="65" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="31">
+        <v>44636</v>
+      </c>
+      <c r="B65" s="18">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C65" s="18">
+        <v>0.34861111111111115</v>
+      </c>
       <c r="D65" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E65" s="30"/>
+        <v>1.5277777777777835E-2</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>128</v>
+      </c>
       <c r="F65" s="23"/>
       <c r="G65" s="19"/>
       <c r="H65" s="20"/>
     </row>
     <row r="66" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0.35625000000000001</v>
+      </c>
       <c r="D66" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E66" s="30"/>
-      <c r="F66" s="21"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>130</v>
+      </c>
       <c r="G66" s="6"/>
       <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
+      <c r="A67" s="31">
+        <v>44636</v>
+      </c>
+      <c r="B67" s="18">
+        <v>0.35625000000000001</v>
+      </c>
+      <c r="C67" s="18">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D67" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E67" s="30"/>
-      <c r="F67" s="23"/>
+        <v>4.3055555555555569E-2</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F67" s="23" t="s">
+        <v>132</v>
+      </c>
       <c r="G67" s="19"/>
       <c r="H67" s="20"/>
     </row>

</xml_diff>